<commit_message>
feat: implement funtionality to download excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -26,25 +26,28 @@
     <t>Servicio</t>
   </si>
   <si>
-    <t>esteban salas</t>
+    <t>fiorella</t>
+  </si>
+  <si>
+    <t>bustamante</t>
+  </si>
+  <si>
+    <t>cámaras</t>
   </si>
   <si>
     <t>internet</t>
   </si>
   <si>
-    <t>lucas rodriguez</t>
-  </si>
-  <si>
-    <t>internet + cable</t>
-  </si>
-  <si>
     <t>Esteban Salas Sulca</t>
   </si>
   <si>
-    <t>juan</t>
-  </si>
-  <si>
-    <t>cámaras</t>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>ge</t>
+  </si>
+  <si>
+    <t>internet_cable</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,41 +410,41 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>9234343434</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
+      <c r="A3">
+        <v>3434</v>
       </c>
       <c r="B3">
-        <v>2342323232</v>
+        <v>344343343</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4">
+        <v>3434</v>
       </c>
       <c r="B4">
-        <v>2342323232</v>
+        <v>34434334</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5">
+        <v>3434</v>
       </c>
       <c r="B5">
-        <v>2342323232</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -455,18 +458,128 @@
         <v>927859435</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>927859435</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>927859435</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>927859435</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>927859435</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>927859435</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>927859435</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>927859435</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>9</v>
+      </c>
+      <c r="B13">
+        <v>927859435</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>927859435</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>927859435</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>927859435</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>927859435</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregar un nuevo campo en el excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Nombre</t>
   </si>
@@ -26,28 +26,16 @@
     <t>Servicio</t>
   </si>
   <si>
-    <t>fiorella</t>
-  </si>
-  <si>
-    <t>bustamante</t>
-  </si>
-  <si>
-    <t>cámaras</t>
-  </si>
-  <si>
-    <t>internet</t>
-  </si>
-  <si>
-    <t>Esteban Salas Sulca</t>
-  </si>
-  <si>
-    <t>cable</t>
-  </si>
-  <si>
-    <t>ge</t>
+    <t>Día y Hora</t>
+  </si>
+  <si>
+    <t>silvanito</t>
   </si>
   <si>
     <t>internet_cable</t>
+  </si>
+  <si>
+    <t>2024-07-07 20:30:23</t>
   </si>
 </sst>
 </file>
@@ -387,7 +375,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,7 +383,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,180 +393,21 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
         <v>4</v>
+      </c>
+      <c r="B2">
+        <v>927859435</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>3434</v>
-      </c>
-      <c r="B3">
-        <v>344343343</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3434</v>
-      </c>
-      <c r="B4">
-        <v>34434334</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>3434</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>927859435</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>927859435</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>927859435</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>927859435</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>927859435</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>927859435</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>927859435</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>927859435</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>927859435</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>927859435</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>927859435</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>927859435</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: impelentar enviar datos al cliente
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -29,13 +29,46 @@
     <t>Día y Hora</t>
   </si>
   <si>
-    <t>silvanito</t>
-  </si>
-  <si>
-    <t>internet_cable</t>
-  </si>
-  <si>
-    <t>2024-07-07 20:30:23</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>2024-07-14 10:36:53</t>
+  </si>
+  <si>
+    <t>jose</t>
+  </si>
+  <si>
+    <t>2024-07-14 10:39:15</t>
+  </si>
+  <si>
+    <t>lucas</t>
+  </si>
+  <si>
+    <t>internet y cable</t>
+  </si>
+  <si>
+    <t>2024-07-14 10:39:42</t>
+  </si>
+  <si>
+    <t>Esteban Salas Sulca</t>
+  </si>
+  <si>
+    <t>cámaras</t>
+  </si>
+  <si>
+    <t>2024-07-14 10:45:19</t>
+  </si>
+  <si>
+    <t>ronal Salas Sulca</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>2024-07-14 14:57:09</t>
   </si>
 </sst>
 </file>
@@ -54,15 +87,27 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +115,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,40 +437,102 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="23.423" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
+        <v>927854934</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1234</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
         <v>927859435</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>927859435</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <v>927859435</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>